<commit_message>
Clase 14 mejores bo
</commit_message>
<xml_diff>
--- a/German/Clase 14/Performance clase 14.xlsx
+++ b/German/Clase 14/Performance clase 14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\Clase 14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA3F37-83E4-4D46-B636-14748E1067BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B5EB5-F4C4-4210-9474-A4DDC15B37AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fechas del Experimento" sheetId="6" r:id="rId1"/>
@@ -1559,6 +1559,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1620,9 +1623,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30051,86 +30051,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="59">
         <v>2019</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="58">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="59">
         <v>2020</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="61">
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="62">
         <v>2021</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="64"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
@@ -30282,13 +30282,13 @@
       <c r="O4" s="48">
         <v>1</v>
       </c>
-      <c r="P4" s="64" t="s">
+      <c r="P4" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="67"/>
       <c r="U4" s="48">
         <v>1</v>
       </c>
@@ -30342,11 +30342,11 @@
       <c r="M5" s="15"/>
       <c r="N5" s="14"/>
       <c r="O5" s="10"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="68"/>
-      <c r="S5" s="68"/>
-      <c r="T5" s="69"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="70"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
@@ -30382,11 +30382,11 @@
       <c r="M6" s="15"/>
       <c r="N6" s="14"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="69"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="70"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
@@ -30446,11 +30446,11 @@
       <c r="O7" s="48">
         <v>1</v>
       </c>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="68"/>
-      <c r="T7" s="69"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="69"/>
+      <c r="S7" s="69"/>
+      <c r="T7" s="70"/>
       <c r="U7" s="48">
         <v>1</v>
       </c>
@@ -30508,11 +30508,11 @@
       <c r="M8" s="18"/>
       <c r="N8" s="16"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="72"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="73"/>
       <c r="U8" s="17"/>
       <c r="V8" s="17"/>
       <c r="W8" s="17"/>
@@ -30600,24 +30600,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="G1" s="74" t="s">
+      <c r="C1" s="75"/>
+      <c r="G1" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="74"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="G2" s="73" t="s">
+      <c r="C2" s="74"/>
+      <c r="G2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -30813,7 +30813,7 @@
       <selection activeCell="E8" sqref="E8"/>
       <selection pane="topRight" activeCell="E8" sqref="E8"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30839,80 +30839,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="Y1" s="74" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="Y1" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="74"/>
-      <c r="AF1" s="74"/>
-      <c r="AG1" s="74"/>
-      <c r="AH1" s="74"/>
-      <c r="AI1" s="74"/>
-      <c r="AJ1" s="74"/>
-      <c r="AK1" s="74"/>
-      <c r="AL1" s="74"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="E2" s="73" t="s">
+      <c r="C2" s="74"/>
+      <c r="E2" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="H2" s="73" t="s">
+      <c r="F2" s="74"/>
+      <c r="H2" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="73"/>
-      <c r="K2" s="73" t="s">
+      <c r="I2" s="74"/>
+      <c r="K2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="N2" s="73" t="s">
+      <c r="L2" s="74"/>
+      <c r="N2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="Y2" s="73" t="s">
+      <c r="O2" s="74"/>
+      <c r="Y2" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="73"/>
-      <c r="AB2" s="73" t="s">
+      <c r="Z2" s="74"/>
+      <c r="AB2" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="73"/>
-      <c r="AE2" s="73" t="s">
+      <c r="AC2" s="74"/>
+      <c r="AE2" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="73"/>
-      <c r="AH2" s="73" t="s">
+      <c r="AF2" s="74"/>
+      <c r="AH2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="73"/>
-      <c r="AK2" s="73" t="s">
+      <c r="AI2" s="74"/>
+      <c r="AK2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="AL2" s="73"/>
+      <c r="AL2" s="74"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -31041,7 +31041,7 @@
       <c r="A7" s="2">
         <v>9500</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="57">
         <v>128.875</v>
       </c>
       <c r="C7" s="3"/>
@@ -31061,7 +31061,7 @@
       <c r="A8" s="2">
         <v>10000</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="57">
         <v>128.315</v>
       </c>
       <c r="C8" s="3"/>
@@ -31081,7 +31081,7 @@
       <c r="A9" s="2">
         <v>10500</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="57">
         <v>124.815</v>
       </c>
       <c r="C9" s="3"/>
@@ -31101,7 +31101,7 @@
       <c r="A10" s="2">
         <v>11000</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="57">
         <v>121.455</v>
       </c>
       <c r="C10" s="3"/>
@@ -31121,7 +31121,7 @@
       <c r="A11" s="2">
         <v>11500</v>
       </c>
-      <c r="B11" s="78">
+      <c r="B11" s="57">
         <v>120.405</v>
       </c>
       <c r="C11" s="3"/>
@@ -31141,7 +31141,7 @@
       <c r="A12" s="2">
         <v>12000</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B12" s="57">
         <v>122.505</v>
       </c>
       <c r="C12" s="3"/>
@@ -31161,7 +31161,7 @@
       <c r="A13" s="2">
         <v>12500</v>
       </c>
-      <c r="B13" s="78">
+      <c r="B13" s="57">
         <v>119.77500000000001</v>
       </c>
       <c r="C13" s="3"/>
@@ -31181,7 +31181,7 @@
       <c r="A14" s="2">
         <v>13000</v>
       </c>
-      <c r="B14" s="78">
+      <c r="B14" s="57">
         <v>116.34399999999999</v>
       </c>
       <c r="C14" s="3"/>
@@ -31201,7 +31201,7 @@
       <c r="A15" s="2">
         <v>13500</v>
       </c>
-      <c r="B15" s="78">
+      <c r="B15" s="57">
         <v>115.994</v>
       </c>
       <c r="C15" s="3"/>
@@ -31366,23 +31366,23 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
       <c r="H1" s="31"/>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
@@ -32713,33 +32713,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="J1" s="77" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="J1" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="T1" s="75" t="s">
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="T1" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="T2" s="20" t="s">
@@ -32763,24 +32763,24 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="J3" s="76" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
       <c r="T3" s="20" t="s">
         <v>60</v>
       </c>
@@ -33648,24 +33648,24 @@
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="J27" s="76" t="s">
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="J27" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="76"/>
-      <c r="N27" s="76"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="76"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="77"/>
+      <c r="N27" s="77"/>
+      <c r="O27" s="77"/>
+      <c r="P27" s="77"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -34427,8 +34427,11 @@
   </sheetPr>
   <dimension ref="A1:AI67"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34651,430 +34654,430 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="22">
         <v>1060</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="22">
         <v>3475627</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="22">
         <v>-100</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="22">
         <v>-1</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="22">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="22">
         <v>0</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="22">
         <v>0</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="22">
         <v>31</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="24">
         <v>561</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="22">
         <v>1</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="22">
         <v>1</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="22">
         <v>1</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="22">
         <v>1</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="22">
         <v>50</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="22">
         <v>279511</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="24">
         <v>295</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="24">
         <v>42234</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="22">
         <v>11603</v>
       </c>
-      <c r="AH3" s="4">
+      <c r="AH3" s="23">
         <v>163984557221389</v>
       </c>
-      <c r="AI3">
+      <c r="AI3" s="22">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="22">
         <v>1060</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="22">
         <v>3475627</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="22">
         <v>-100</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="22">
         <v>-1</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="22">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="22">
         <v>0</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="22">
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="22">
         <v>31</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="24">
         <v>2147</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="22">
         <v>1</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="22">
         <v>1</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="22">
         <v>1</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="22">
         <v>1</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="22">
         <v>50</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="22">
         <v>279511</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="24">
         <v>331</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="24">
         <v>22431</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="22">
         <v>11483</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AH4" s="23">
         <v>163900739130435</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="22">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="22">
         <v>1060</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="22">
         <v>3475627</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="22">
         <v>-100</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="22">
         <v>-1</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="22">
         <v>0</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="22">
         <v>0</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="22">
         <v>0</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="22">
         <v>31</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="24">
         <v>799</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="22">
         <v>1</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="22">
         <v>1</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="22">
         <v>1</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="22">
         <v>1</v>
       </c>
-      <c r="X5" t="s">
+      <c r="X5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="22">
         <v>50</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AA5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="22">
         <v>279511</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AC5" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="24">
         <v>247</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="24">
         <v>49996</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="22">
         <v>13296</v>
       </c>
-      <c r="AH5" s="4">
+      <c r="AH5" s="23">
         <v>162908729635182</v>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="22">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="22">
         <v>1060</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="22">
         <v>3475627</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="22">
         <v>-100</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="22">
         <v>-1</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="22">
         <v>0</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="22">
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="22">
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="22">
         <v>31</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="24">
         <v>2985</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="22">
         <v>1</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="22">
         <v>1</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="22">
         <v>1</v>
       </c>
-      <c r="V6" t="s">
+      <c r="V6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="22">
         <v>1</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="22">
         <v>50</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="Z6" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="22">
         <v>279511</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AC6" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="24">
         <v>356</v>
       </c>
-      <c r="AF6">
+      <c r="AF6" s="24">
         <v>49985</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="22">
         <v>12615</v>
       </c>
-      <c r="AH6" s="4">
+      <c r="AH6" s="23">
         <v>162833170914543</v>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="22">
         <v>25</v>
       </c>
     </row>

</xml_diff>